<commit_message>
Updated screenshots and content
</commit_message>
<xml_diff>
--- a/_templates/Operational_Logistics_Board/Jobs_Positions_de.xlsx
+++ b/_templates/Operational_Logistics_Board/Jobs_Positions_de.xlsx
@@ -8,26 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiashaas/git/peakboard-templates/_templates/Operational_Logistics_Board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9C6630-6EDD-EE48-98D2-2A3CAC9E4F24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D36B50-7943-D541-9FAC-D5A546D5F621}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-40620" yWindow="-4960" windowWidth="36780" windowHeight="28080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$F$61</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="66">
   <si>
     <t>job</t>
   </si>
   <si>
-    <t>Manual</t>
-  </si>
-  <si>
     <t>area_code</t>
   </si>
   <si>
@@ -43,9 +43,6 @@
     <t>Small Parts</t>
   </si>
   <si>
-    <t>High Rack</t>
-  </si>
-  <si>
     <t>part_title</t>
   </si>
   <si>
@@ -215,6 +212,15 @@
   </si>
   <si>
     <t>Kuchen - Kasten</t>
+  </si>
+  <si>
+    <t>Manuell</t>
+  </si>
+  <si>
+    <t>Kleinteile</t>
+  </si>
+  <si>
+    <t>Hochregal</t>
   </si>
 </sst>
 </file>
@@ -575,7 +581,7 @@
   <dimension ref="A1:F869"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -593,19 +599,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
@@ -616,7 +622,7 @@
         <v>100</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="D2" s="2">
         <v>300</v>
@@ -625,7 +631,7 @@
         <v>300</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
@@ -636,7 +642,7 @@
         <v>100</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="D3" s="2">
         <v>250</v>
@@ -645,7 +651,7 @@
         <v>80</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
@@ -656,7 +662,7 @@
         <v>100</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="D4" s="2">
         <v>260</v>
@@ -665,7 +671,7 @@
         <v>63</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -676,7 +682,7 @@
         <v>200</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="D5" s="2">
         <v>2000</v>
@@ -685,7 +691,7 @@
         <v>1200</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
@@ -696,7 +702,7 @@
         <v>200</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="D6" s="2">
         <v>1600</v>
@@ -705,7 +711,7 @@
         <v>1400</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
@@ -716,7 +722,7 @@
         <v>200</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="D7" s="2">
         <v>2300</v>
@@ -725,7 +731,7 @@
         <v>1600</v>
       </c>
       <c r="F7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
@@ -736,7 +742,7 @@
         <v>200</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="D8" s="2">
         <v>1600</v>
@@ -745,7 +751,7 @@
         <v>200</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
@@ -756,7 +762,7 @@
         <v>300</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D9" s="2">
         <v>20</v>
@@ -765,7 +771,7 @@
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
@@ -776,7 +782,7 @@
         <v>300</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D10" s="2">
         <v>26</v>
@@ -785,7 +791,7 @@
         <v>26</v>
       </c>
       <c r="F10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
@@ -796,7 +802,7 @@
         <v>300</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D11" s="2">
         <v>28</v>
@@ -805,7 +811,7 @@
         <v>28</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
@@ -816,7 +822,7 @@
         <v>300</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D12" s="2">
         <v>33</v>
@@ -825,7 +831,7 @@
         <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
@@ -836,7 +842,7 @@
         <v>300</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D13" s="2">
         <v>13</v>
@@ -845,7 +851,7 @@
         <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
@@ -856,7 +862,7 @@
         <v>300</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D14" s="2">
         <v>48</v>
@@ -865,7 +871,7 @@
         <v>42</v>
       </c>
       <c r="F14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
@@ -876,7 +882,7 @@
         <v>300</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D15" s="2">
         <v>72</v>
@@ -885,7 +891,7 @@
         <v>60</v>
       </c>
       <c r="F15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
@@ -896,7 +902,7 @@
         <v>300</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D16" s="2">
         <v>36</v>
@@ -905,7 +911,7 @@
         <v>36</v>
       </c>
       <c r="F16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
@@ -916,7 +922,7 @@
         <v>100</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="D17" s="2">
         <v>160</v>
@@ -925,7 +931,7 @@
         <v>160</v>
       </c>
       <c r="F17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
@@ -936,7 +942,7 @@
         <v>200</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="D18" s="2">
         <v>1600</v>
@@ -945,7 +951,7 @@
         <v>1600</v>
       </c>
       <c r="F18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
@@ -956,7 +962,7 @@
         <v>200</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="D19" s="2">
         <v>1200</v>
@@ -965,7 +971,7 @@
         <v>800</v>
       </c>
       <c r="F19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
@@ -976,7 +982,7 @@
         <v>200</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="D20" s="2">
         <v>800</v>
@@ -985,7 +991,7 @@
         <v>600</v>
       </c>
       <c r="F20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
@@ -996,7 +1002,7 @@
         <v>300</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D21" s="2">
         <v>120</v>
@@ -1005,7 +1011,7 @@
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
@@ -1016,7 +1022,7 @@
         <v>300</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D22" s="2">
         <v>86</v>
@@ -1025,7 +1031,7 @@
         <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
@@ -1036,7 +1042,7 @@
         <v>300</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D23" s="2">
         <v>23</v>
@@ -1045,7 +1051,7 @@
         <v>23</v>
       </c>
       <c r="F23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
@@ -1056,7 +1062,7 @@
         <v>300</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D24" s="2">
         <v>12</v>
@@ -1065,7 +1071,7 @@
         <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
@@ -1076,7 +1082,7 @@
         <v>100</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="D25" s="2">
         <v>260</v>
@@ -1085,7 +1091,7 @@
         <v>120</v>
       </c>
       <c r="F25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
@@ -1096,7 +1102,7 @@
         <v>100</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="D26" s="2">
         <v>240</v>
@@ -1105,7 +1111,7 @@
         <v>100</v>
       </c>
       <c r="F26" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
@@ -1116,7 +1122,7 @@
         <v>100</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="D27" s="2">
         <v>180</v>
@@ -1125,7 +1131,7 @@
         <v>20</v>
       </c>
       <c r="F27" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
@@ -1136,7 +1142,7 @@
         <v>100</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="D28" s="2">
         <v>260</v>
@@ -1145,7 +1151,7 @@
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
@@ -1156,7 +1162,7 @@
         <v>100</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="D29" s="2">
         <v>120</v>
@@ -1165,7 +1171,7 @@
         <v>120</v>
       </c>
       <c r="F29" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
@@ -1176,7 +1182,7 @@
         <v>100</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="D30" s="2">
         <v>300</v>
@@ -1185,7 +1191,7 @@
         <v>160</v>
       </c>
       <c r="F30" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
@@ -1196,7 +1202,7 @@
         <v>100</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="D31" s="2">
         <v>180</v>
@@ -1205,7 +1211,7 @@
         <v>120</v>
       </c>
       <c r="F31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
@@ -1216,7 +1222,7 @@
         <v>200</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="D32" s="2">
         <v>800</v>
@@ -1225,7 +1231,7 @@
         <v>60</v>
       </c>
       <c r="F32" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
@@ -1236,7 +1242,7 @@
         <v>200</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="D33" s="2">
         <v>650</v>
@@ -1245,7 +1251,7 @@
         <v>160</v>
       </c>
       <c r="F33" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
@@ -1256,7 +1262,7 @@
         <v>200</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="D34" s="2">
         <v>3560</v>
@@ -1265,7 +1271,7 @@
         <v>3000</v>
       </c>
       <c r="F34" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
@@ -1276,7 +1282,7 @@
         <v>200</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="D35" s="2">
         <v>8600</v>
@@ -1285,7 +1291,7 @@
         <v>100</v>
       </c>
       <c r="F35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
@@ -1296,7 +1302,7 @@
         <v>300</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D36" s="2">
         <v>30</v>
@@ -1305,7 +1311,7 @@
         <v>2</v>
       </c>
       <c r="F36" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
@@ -1316,7 +1322,7 @@
         <v>300</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D37" s="2">
         <v>76</v>
@@ -1325,7 +1331,7 @@
         <v>4</v>
       </c>
       <c r="F37" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
@@ -1336,7 +1342,7 @@
         <v>300</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D38" s="2">
         <v>91</v>
@@ -1345,7 +1351,7 @@
         <v>6</v>
       </c>
       <c r="F38" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
@@ -1356,7 +1362,7 @@
         <v>300</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D39" s="2">
         <v>90</v>
@@ -1365,7 +1371,7 @@
         <v>0</v>
       </c>
       <c r="F39" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
@@ -1376,14 +1382,14 @@
         <v>100</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="D40" s="2">
         <v>120</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
@@ -1394,14 +1400,14 @@
         <v>200</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D41" s="2">
         <v>600</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
@@ -1412,14 +1418,14 @@
         <v>200</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D42" s="2">
         <v>1600</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
@@ -1430,14 +1436,14 @@
         <v>200</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D43" s="2">
         <v>1200</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
@@ -1448,14 +1454,14 @@
         <v>300</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D44" s="2">
         <v>800</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
@@ -1466,14 +1472,14 @@
         <v>300</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D45" s="2">
         <v>120</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
@@ -1484,14 +1490,14 @@
         <v>300</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D46" s="2">
         <v>86</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
@@ -1502,14 +1508,14 @@
         <v>300</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D47" s="2">
         <v>23</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.15">
@@ -1520,14 +1526,14 @@
         <v>300</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D48" s="2">
         <v>12</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
@@ -1538,14 +1544,14 @@
         <v>300</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D49" s="2">
         <v>26</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
@@ -1556,14 +1562,14 @@
         <v>300</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D50" s="2">
         <v>24</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
@@ -1574,14 +1580,14 @@
         <v>300</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D51" s="2">
         <v>18</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
@@ -1592,14 +1598,14 @@
         <v>100</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="D52" s="2">
         <v>260</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
@@ -1610,14 +1616,14 @@
         <v>100</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="D53" s="2">
         <v>120</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
@@ -1628,14 +1634,14 @@
         <v>100</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="D54" s="2">
         <v>300</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
@@ -1646,14 +1652,14 @@
         <v>100</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="D55" s="2">
         <v>180</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
@@ -1664,14 +1670,14 @@
         <v>100</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="D56" s="2">
         <v>800</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
@@ -1682,14 +1688,14 @@
         <v>200</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D57" s="2">
         <v>650</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
@@ -1700,14 +1706,14 @@
         <v>200</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D58" s="2">
         <v>3560</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
@@ -1718,14 +1724,14 @@
         <v>200</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D59" s="2">
         <v>8600</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
@@ -1736,14 +1742,14 @@
         <v>300</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D60" s="2">
         <v>30</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
@@ -1754,14 +1760,14 @@
         <v>300</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D61" s="2">
         <v>76</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
@@ -4195,6 +4201,7 @@
       <c r="A869" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F61" xr:uid="{37838DC9-7F13-D643-896D-E8964E5ECCC3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A869">
     <sortCondition descending="1" ref="A1"/>
   </sortState>

</xml_diff>